<commit_message>
Day 4 not Day 2
</commit_message>
<xml_diff>
--- a/Advent-of-code-2023-Excel.xlsx
+++ b/Advent-of-code-2023-Excel.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8508653-4677-444D-89F7-52C5C0D3839F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D4909BD-6EA2-4B56-A1A5-6FA90D309F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D1-Solution" sheetId="1" r:id="rId1"/>
     <sheet name="D1-Input" sheetId="2" r:id="rId2"/>
-    <sheet name="D2-Solution" sheetId="4" r:id="rId3"/>
-    <sheet name="D2-Input" sheetId="3" r:id="rId4"/>
+    <sheet name="D4-Solution" sheetId="4" r:id="rId3"/>
+    <sheet name="D4-Input" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -3061,7 +3061,7 @@
     <t>3nine6five1</t>
   </si>
   <si>
-    <t>Day 2</t>
+    <t>Day 4</t>
   </si>
   <si>
     <t>Winning numbers</t>
@@ -15456,8 +15456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE0EA68-8CD6-4D32-8A61-F34D66C02A36}">
   <dimension ref="A1:AR214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AR10" sqref="AR10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15491,7 +15491,7 @@
     </row>
     <row r="3" spans="1:44">
       <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3:P3">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A3)," ")</f>
+        <f t="array" ref="A3:P3">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A3)," ")</f>
         <v>Card</v>
       </c>
       <c r="B3" t="str">
@@ -15555,7 +15555,7 @@
     </row>
     <row r="4" spans="1:44">
       <c r="A4" t="str" cm="1">
-        <f t="array" ref="A4:P4">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A4)," ")</f>
+        <f t="array" ref="A4:P4">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A4)," ")</f>
         <v>Card</v>
       </c>
       <c r="B4" t="str">
@@ -15614,7 +15614,7 @@
     </row>
     <row r="5" spans="1:44">
       <c r="A5" t="str" cm="1">
-        <f t="array" ref="A5:P5">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A5)," ")</f>
+        <f t="array" ref="A5:P5">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A5)," ")</f>
         <v>Card</v>
       </c>
       <c r="B5" t="str">
@@ -15678,7 +15678,7 @@
     </row>
     <row r="6" spans="1:44">
       <c r="A6" t="str" cm="1">
-        <f t="array" ref="A6:P6">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A6)," ")</f>
+        <f t="array" ref="A6:P6">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A6)," ")</f>
         <v>Card</v>
       </c>
       <c r="B6" t="str">
@@ -15737,7 +15737,7 @@
     </row>
     <row r="7" spans="1:44">
       <c r="A7" t="str" cm="1">
-        <f t="array" ref="A7:P7">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A7)," ")</f>
+        <f t="array" ref="A7:P7">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A7)," ")</f>
         <v>Card</v>
       </c>
       <c r="B7" t="str">
@@ -15796,7 +15796,7 @@
     </row>
     <row r="8" spans="1:44">
       <c r="A8" t="str" cm="1">
-        <f t="array" ref="A8:P8">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A8)," ")</f>
+        <f t="array" ref="A8:P8">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A8)," ")</f>
         <v>Card</v>
       </c>
       <c r="B8" t="str">
@@ -15863,7 +15863,7 @@
     </row>
     <row r="11" spans="1:44">
       <c r="A11" t="str" cm="1">
-        <f t="array" ref="A11:AL11">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A11)," ")</f>
+        <f t="array" ref="A11:AL11">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A11)," ")</f>
         <v>Card</v>
       </c>
       <c r="B11" t="str">
@@ -15992,7 +15992,7 @@
     </row>
     <row r="12" spans="1:44">
       <c r="A12" t="str" cm="1">
-        <f t="array" ref="A12:AL12">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A12)," ")</f>
+        <f t="array" ref="A12:AL12">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A12)," ")</f>
         <v>Card</v>
       </c>
       <c r="B12" t="str">
@@ -16117,7 +16117,7 @@
     </row>
     <row r="13" spans="1:44">
       <c r="A13" t="str" cm="1">
-        <f t="array" ref="A13:AL13">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A13)," ")</f>
+        <f t="array" ref="A13:AL13">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A13)," ")</f>
         <v>Card</v>
       </c>
       <c r="B13" t="str">
@@ -16242,7 +16242,7 @@
     </row>
     <row r="14" spans="1:44">
       <c r="A14" t="str" cm="1">
-        <f t="array" ref="A14:AL14">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A14)," ")</f>
+        <f t="array" ref="A14:AL14">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A14)," ")</f>
         <v>Card</v>
       </c>
       <c r="B14" t="str">
@@ -16367,7 +16367,7 @@
     </row>
     <row r="15" spans="1:44">
       <c r="A15" t="str" cm="1">
-        <f t="array" ref="A15:AL15">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A15)," ")</f>
+        <f t="array" ref="A15:AL15">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A15)," ")</f>
         <v>Card</v>
       </c>
       <c r="B15" t="str">
@@ -16492,7 +16492,7 @@
     </row>
     <row r="16" spans="1:44">
       <c r="A16" t="str" cm="1">
-        <f t="array" ref="A16:AL16">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A16)," ")</f>
+        <f t="array" ref="A16:AL16">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A16)," ")</f>
         <v>Card</v>
       </c>
       <c r="B16" t="str">
@@ -16617,7 +16617,7 @@
     </row>
     <row r="17" spans="1:42">
       <c r="A17" t="str" cm="1">
-        <f t="array" ref="A17:AL17">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A17)," ")</f>
+        <f t="array" ref="A17:AL17">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A17)," ")</f>
         <v>Card</v>
       </c>
       <c r="B17" t="str">
@@ -16742,7 +16742,7 @@
     </row>
     <row r="18" spans="1:42">
       <c r="A18" t="str" cm="1">
-        <f t="array" ref="A18:AL18">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A18)," ")</f>
+        <f t="array" ref="A18:AL18">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A18)," ")</f>
         <v>Card</v>
       </c>
       <c r="B18" t="str">
@@ -16867,7 +16867,7 @@
     </row>
     <row r="19" spans="1:42">
       <c r="A19" t="str" cm="1">
-        <f t="array" ref="A19:AL19">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A19)," ")</f>
+        <f t="array" ref="A19:AL19">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A19)," ")</f>
         <v>Card</v>
       </c>
       <c r="B19" t="str">
@@ -16992,7 +16992,7 @@
     </row>
     <row r="20" spans="1:42">
       <c r="A20" t="str" cm="1">
-        <f t="array" ref="A20:AL20">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A20)," ")</f>
+        <f t="array" ref="A20:AL20">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A20)," ")</f>
         <v>Card</v>
       </c>
       <c r="B20" t="str">
@@ -17117,7 +17117,7 @@
     </row>
     <row r="21" spans="1:42">
       <c r="A21" t="str" cm="1">
-        <f t="array" ref="A21:AL21">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A21)," ")</f>
+        <f t="array" ref="A21:AL21">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A21)," ")</f>
         <v>Card</v>
       </c>
       <c r="B21" t="str">
@@ -17242,7 +17242,7 @@
     </row>
     <row r="22" spans="1:42">
       <c r="A22" t="str" cm="1">
-        <f t="array" ref="A22:AL22">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A22)," ")</f>
+        <f t="array" ref="A22:AL22">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A22)," ")</f>
         <v>Card</v>
       </c>
       <c r="B22" t="str">
@@ -17367,7 +17367,7 @@
     </row>
     <row r="23" spans="1:42">
       <c r="A23" t="str" cm="1">
-        <f t="array" ref="A23:AL23">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A23)," ")</f>
+        <f t="array" ref="A23:AL23">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A23)," ")</f>
         <v>Card</v>
       </c>
       <c r="B23" t="str">
@@ -17492,7 +17492,7 @@
     </row>
     <row r="24" spans="1:42">
       <c r="A24" t="str" cm="1">
-        <f t="array" ref="A24:AL24">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A24)," ")</f>
+        <f t="array" ref="A24:AL24">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A24)," ")</f>
         <v>Card</v>
       </c>
       <c r="B24" t="str">
@@ -17617,7 +17617,7 @@
     </row>
     <row r="25" spans="1:42">
       <c r="A25" t="str" cm="1">
-        <f t="array" ref="A25:AL25">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A25)," ")</f>
+        <f t="array" ref="A25:AL25">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A25)," ")</f>
         <v>Card</v>
       </c>
       <c r="B25" t="str">
@@ -17742,7 +17742,7 @@
     </row>
     <row r="26" spans="1:42">
       <c r="A26" t="str" cm="1">
-        <f t="array" ref="A26:AL26">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A26)," ")</f>
+        <f t="array" ref="A26:AL26">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A26)," ")</f>
         <v>Card</v>
       </c>
       <c r="B26" t="str">
@@ -17867,7 +17867,7 @@
     </row>
     <row r="27" spans="1:42">
       <c r="A27" t="str" cm="1">
-        <f t="array" ref="A27:AL27">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A27)," ")</f>
+        <f t="array" ref="A27:AL27">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A27)," ")</f>
         <v>Card</v>
       </c>
       <c r="B27" t="str">
@@ -17992,7 +17992,7 @@
     </row>
     <row r="28" spans="1:42">
       <c r="A28" t="str" cm="1">
-        <f t="array" ref="A28:AL28">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A28)," ")</f>
+        <f t="array" ref="A28:AL28">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A28)," ")</f>
         <v>Card</v>
       </c>
       <c r="B28" t="str">
@@ -18117,7 +18117,7 @@
     </row>
     <row r="29" spans="1:42">
       <c r="A29" t="str" cm="1">
-        <f t="array" ref="A29:AL29">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A29)," ")</f>
+        <f t="array" ref="A29:AL29">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A29)," ")</f>
         <v>Card</v>
       </c>
       <c r="B29" t="str">
@@ -18242,7 +18242,7 @@
     </row>
     <row r="30" spans="1:42">
       <c r="A30" t="str" cm="1">
-        <f t="array" ref="A30:AL30">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A30)," ")</f>
+        <f t="array" ref="A30:AL30">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A30)," ")</f>
         <v>Card</v>
       </c>
       <c r="B30" t="str">
@@ -18367,7 +18367,7 @@
     </row>
     <row r="31" spans="1:42">
       <c r="A31" t="str" cm="1">
-        <f t="array" ref="A31:AL31">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A31)," ")</f>
+        <f t="array" ref="A31:AL31">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A31)," ")</f>
         <v>Card</v>
       </c>
       <c r="B31" t="str">
@@ -18492,7 +18492,7 @@
     </row>
     <row r="32" spans="1:42">
       <c r="A32" t="str" cm="1">
-        <f t="array" ref="A32:AL32">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A32)," ")</f>
+        <f t="array" ref="A32:AL32">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A32)," ")</f>
         <v>Card</v>
       </c>
       <c r="B32" t="str">
@@ -18617,7 +18617,7 @@
     </row>
     <row r="33" spans="1:42">
       <c r="A33" t="str" cm="1">
-        <f t="array" ref="A33:AL33">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A33)," ")</f>
+        <f t="array" ref="A33:AL33">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A33)," ")</f>
         <v>Card</v>
       </c>
       <c r="B33" t="str">
@@ -18742,7 +18742,7 @@
     </row>
     <row r="34" spans="1:42">
       <c r="A34" t="str" cm="1">
-        <f t="array" ref="A34:AL34">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A34)," ")</f>
+        <f t="array" ref="A34:AL34">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A34)," ")</f>
         <v>Card</v>
       </c>
       <c r="B34" t="str">
@@ -18867,7 +18867,7 @@
     </row>
     <row r="35" spans="1:42">
       <c r="A35" t="str" cm="1">
-        <f t="array" ref="A35:AL35">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A35)," ")</f>
+        <f t="array" ref="A35:AL35">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A35)," ")</f>
         <v>Card</v>
       </c>
       <c r="B35" t="str">
@@ -18992,7 +18992,7 @@
     </row>
     <row r="36" spans="1:42">
       <c r="A36" t="str" cm="1">
-        <f t="array" ref="A36:AL36">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A36)," ")</f>
+        <f t="array" ref="A36:AL36">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A36)," ")</f>
         <v>Card</v>
       </c>
       <c r="B36" t="str">
@@ -19117,7 +19117,7 @@
     </row>
     <row r="37" spans="1:42">
       <c r="A37" t="str" cm="1">
-        <f t="array" ref="A37:AL37">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A37)," ")</f>
+        <f t="array" ref="A37:AL37">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A37)," ")</f>
         <v>Card</v>
       </c>
       <c r="B37" t="str">
@@ -19242,7 +19242,7 @@
     </row>
     <row r="38" spans="1:42">
       <c r="A38" t="str" cm="1">
-        <f t="array" ref="A38:AL38">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A38)," ")</f>
+        <f t="array" ref="A38:AL38">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A38)," ")</f>
         <v>Card</v>
       </c>
       <c r="B38" t="str">
@@ -19367,7 +19367,7 @@
     </row>
     <row r="39" spans="1:42">
       <c r="A39" t="str" cm="1">
-        <f t="array" ref="A39:AL39">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A39)," ")</f>
+        <f t="array" ref="A39:AL39">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A39)," ")</f>
         <v>Card</v>
       </c>
       <c r="B39" t="str">
@@ -19492,7 +19492,7 @@
     </row>
     <row r="40" spans="1:42">
       <c r="A40" t="str" cm="1">
-        <f t="array" ref="A40:AL40">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A40)," ")</f>
+        <f t="array" ref="A40:AL40">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A40)," ")</f>
         <v>Card</v>
       </c>
       <c r="B40" t="str">
@@ -19617,7 +19617,7 @@
     </row>
     <row r="41" spans="1:42">
       <c r="A41" t="str" cm="1">
-        <f t="array" ref="A41:AL41">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A41)," ")</f>
+        <f t="array" ref="A41:AL41">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A41)," ")</f>
         <v>Card</v>
       </c>
       <c r="B41" t="str">
@@ -19742,7 +19742,7 @@
     </row>
     <row r="42" spans="1:42">
       <c r="A42" t="str" cm="1">
-        <f t="array" ref="A42:AL42">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A42)," ")</f>
+        <f t="array" ref="A42:AL42">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A42)," ")</f>
         <v>Card</v>
       </c>
       <c r="B42" t="str">
@@ -19867,7 +19867,7 @@
     </row>
     <row r="43" spans="1:42">
       <c r="A43" t="str" cm="1">
-        <f t="array" ref="A43:AL43">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A43)," ")</f>
+        <f t="array" ref="A43:AL43">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A43)," ")</f>
         <v>Card</v>
       </c>
       <c r="B43" t="str">
@@ -19992,7 +19992,7 @@
     </row>
     <row r="44" spans="1:42">
       <c r="A44" t="str" cm="1">
-        <f t="array" ref="A44:AL44">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A44)," ")</f>
+        <f t="array" ref="A44:AL44">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A44)," ")</f>
         <v>Card</v>
       </c>
       <c r="B44" t="str">
@@ -20117,7 +20117,7 @@
     </row>
     <row r="45" spans="1:42">
       <c r="A45" t="str" cm="1">
-        <f t="array" ref="A45:AL45">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A45)," ")</f>
+        <f t="array" ref="A45:AL45">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A45)," ")</f>
         <v>Card</v>
       </c>
       <c r="B45" t="str">
@@ -20242,7 +20242,7 @@
     </row>
     <row r="46" spans="1:42">
       <c r="A46" t="str" cm="1">
-        <f t="array" ref="A46:AL46">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A46)," ")</f>
+        <f t="array" ref="A46:AL46">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A46)," ")</f>
         <v>Card</v>
       </c>
       <c r="B46" t="str">
@@ -20367,7 +20367,7 @@
     </row>
     <row r="47" spans="1:42">
       <c r="A47" t="str" cm="1">
-        <f t="array" ref="A47:AL47">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A47)," ")</f>
+        <f t="array" ref="A47:AL47">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A47)," ")</f>
         <v>Card</v>
       </c>
       <c r="B47" t="str">
@@ -20492,7 +20492,7 @@
     </row>
     <row r="48" spans="1:42">
       <c r="A48" t="str" cm="1">
-        <f t="array" ref="A48:AL48">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A48)," ")</f>
+        <f t="array" ref="A48:AL48">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A48)," ")</f>
         <v>Card</v>
       </c>
       <c r="B48" t="str">
@@ -20617,7 +20617,7 @@
     </row>
     <row r="49" spans="1:42">
       <c r="A49" t="str" cm="1">
-        <f t="array" ref="A49:AL49">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A49)," ")</f>
+        <f t="array" ref="A49:AL49">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A49)," ")</f>
         <v>Card</v>
       </c>
       <c r="B49" t="str">
@@ -20742,7 +20742,7 @@
     </row>
     <row r="50" spans="1:42">
       <c r="A50" t="str" cm="1">
-        <f t="array" ref="A50:AL50">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A50)," ")</f>
+        <f t="array" ref="A50:AL50">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A50)," ")</f>
         <v>Card</v>
       </c>
       <c r="B50" t="str">
@@ -20867,7 +20867,7 @@
     </row>
     <row r="51" spans="1:42">
       <c r="A51" t="str" cm="1">
-        <f t="array" ref="A51:AL51">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A51)," ")</f>
+        <f t="array" ref="A51:AL51">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A51)," ")</f>
         <v>Card</v>
       </c>
       <c r="B51" t="str">
@@ -20992,7 +20992,7 @@
     </row>
     <row r="52" spans="1:42">
       <c r="A52" t="str" cm="1">
-        <f t="array" ref="A52:AL52">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A52)," ")</f>
+        <f t="array" ref="A52:AL52">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A52)," ")</f>
         <v>Card</v>
       </c>
       <c r="B52" t="str">
@@ -21117,7 +21117,7 @@
     </row>
     <row r="53" spans="1:42">
       <c r="A53" t="str" cm="1">
-        <f t="array" ref="A53:AL53">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A53)," ")</f>
+        <f t="array" ref="A53:AL53">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A53)," ")</f>
         <v>Card</v>
       </c>
       <c r="B53" t="str">
@@ -21242,7 +21242,7 @@
     </row>
     <row r="54" spans="1:42">
       <c r="A54" t="str" cm="1">
-        <f t="array" ref="A54:AL54">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A54)," ")</f>
+        <f t="array" ref="A54:AL54">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A54)," ")</f>
         <v>Card</v>
       </c>
       <c r="B54" t="str">
@@ -21367,7 +21367,7 @@
     </row>
     <row r="55" spans="1:42">
       <c r="A55" t="str" cm="1">
-        <f t="array" ref="A55:AL55">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A55)," ")</f>
+        <f t="array" ref="A55:AL55">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A55)," ")</f>
         <v>Card</v>
       </c>
       <c r="B55" t="str">
@@ -21492,7 +21492,7 @@
     </row>
     <row r="56" spans="1:42">
       <c r="A56" t="str" cm="1">
-        <f t="array" ref="A56:AL56">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A56)," ")</f>
+        <f t="array" ref="A56:AL56">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A56)," ")</f>
         <v>Card</v>
       </c>
       <c r="B56" t="str">
@@ -21617,7 +21617,7 @@
     </row>
     <row r="57" spans="1:42">
       <c r="A57" t="str" cm="1">
-        <f t="array" ref="A57:AL57">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A57)," ")</f>
+        <f t="array" ref="A57:AL57">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A57)," ")</f>
         <v>Card</v>
       </c>
       <c r="B57" t="str">
@@ -21742,7 +21742,7 @@
     </row>
     <row r="58" spans="1:42">
       <c r="A58" t="str" cm="1">
-        <f t="array" ref="A58:AL58">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A58)," ")</f>
+        <f t="array" ref="A58:AL58">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A58)," ")</f>
         <v>Card</v>
       </c>
       <c r="B58" t="str">
@@ -21867,7 +21867,7 @@
     </row>
     <row r="59" spans="1:42">
       <c r="A59" t="str" cm="1">
-        <f t="array" ref="A59:AL59">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A59)," ")</f>
+        <f t="array" ref="A59:AL59">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A59)," ")</f>
         <v>Card</v>
       </c>
       <c r="B59" t="str">
@@ -21992,7 +21992,7 @@
     </row>
     <row r="60" spans="1:42">
       <c r="A60" t="str" cm="1">
-        <f t="array" ref="A60:AL60">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A60)," ")</f>
+        <f t="array" ref="A60:AL60">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A60)," ")</f>
         <v>Card</v>
       </c>
       <c r="B60" t="str">
@@ -22117,7 +22117,7 @@
     </row>
     <row r="61" spans="1:42">
       <c r="A61" t="str" cm="1">
-        <f t="array" ref="A61:AL61">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A61)," ")</f>
+        <f t="array" ref="A61:AL61">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A61)," ")</f>
         <v>Card</v>
       </c>
       <c r="B61" t="str">
@@ -22242,7 +22242,7 @@
     </row>
     <row r="62" spans="1:42">
       <c r="A62" t="str" cm="1">
-        <f t="array" ref="A62:AL62">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A62)," ")</f>
+        <f t="array" ref="A62:AL62">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A62)," ")</f>
         <v>Card</v>
       </c>
       <c r="B62" t="str">
@@ -22367,7 +22367,7 @@
     </row>
     <row r="63" spans="1:42">
       <c r="A63" t="str" cm="1">
-        <f t="array" ref="A63:AL63">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A63)," ")</f>
+        <f t="array" ref="A63:AL63">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A63)," ")</f>
         <v>Card</v>
       </c>
       <c r="B63" t="str">
@@ -22492,7 +22492,7 @@
     </row>
     <row r="64" spans="1:42">
       <c r="A64" t="str" cm="1">
-        <f t="array" ref="A64:AL64">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A64)," ")</f>
+        <f t="array" ref="A64:AL64">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A64)," ")</f>
         <v>Card</v>
       </c>
       <c r="B64" t="str">
@@ -22617,7 +22617,7 @@
     </row>
     <row r="65" spans="1:42">
       <c r="A65" t="str" cm="1">
-        <f t="array" ref="A65:AL65">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A65)," ")</f>
+        <f t="array" ref="A65:AL65">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A65)," ")</f>
         <v>Card</v>
       </c>
       <c r="B65" t="str">
@@ -22742,7 +22742,7 @@
     </row>
     <row r="66" spans="1:42">
       <c r="A66" t="str" cm="1">
-        <f t="array" ref="A66:AL66">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A66)," ")</f>
+        <f t="array" ref="A66:AL66">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A66)," ")</f>
         <v>Card</v>
       </c>
       <c r="B66" t="str">
@@ -22867,7 +22867,7 @@
     </row>
     <row r="67" spans="1:42">
       <c r="A67" t="str" cm="1">
-        <f t="array" ref="A67:AL67">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A67)," ")</f>
+        <f t="array" ref="A67:AL67">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A67)," ")</f>
         <v>Card</v>
       </c>
       <c r="B67" t="str">
@@ -22992,7 +22992,7 @@
     </row>
     <row r="68" spans="1:42">
       <c r="A68" t="str" cm="1">
-        <f t="array" ref="A68:AL68">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A68)," ")</f>
+        <f t="array" ref="A68:AL68">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A68)," ")</f>
         <v>Card</v>
       </c>
       <c r="B68" t="str">
@@ -23117,7 +23117,7 @@
     </row>
     <row r="69" spans="1:42">
       <c r="A69" t="str" cm="1">
-        <f t="array" ref="A69:AL69">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A69)," ")</f>
+        <f t="array" ref="A69:AL69">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A69)," ")</f>
         <v>Card</v>
       </c>
       <c r="B69" t="str">
@@ -23242,7 +23242,7 @@
     </row>
     <row r="70" spans="1:42">
       <c r="A70" t="str" cm="1">
-        <f t="array" ref="A70:AL70">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A70)," ")</f>
+        <f t="array" ref="A70:AL70">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A70)," ")</f>
         <v>Card</v>
       </c>
       <c r="B70" t="str">
@@ -23367,7 +23367,7 @@
     </row>
     <row r="71" spans="1:42">
       <c r="A71" t="str" cm="1">
-        <f t="array" ref="A71:AL71">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A71)," ")</f>
+        <f t="array" ref="A71:AL71">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A71)," ")</f>
         <v>Card</v>
       </c>
       <c r="B71" t="str">
@@ -23492,7 +23492,7 @@
     </row>
     <row r="72" spans="1:42">
       <c r="A72" t="str" cm="1">
-        <f t="array" ref="A72:AL72">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A72)," ")</f>
+        <f t="array" ref="A72:AL72">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A72)," ")</f>
         <v>Card</v>
       </c>
       <c r="B72" t="str">
@@ -23617,7 +23617,7 @@
     </row>
     <row r="73" spans="1:42">
       <c r="A73" t="str" cm="1">
-        <f t="array" ref="A73:AL73">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A73)," ")</f>
+        <f t="array" ref="A73:AL73">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A73)," ")</f>
         <v>Card</v>
       </c>
       <c r="B73" t="str">
@@ -23742,7 +23742,7 @@
     </row>
     <row r="74" spans="1:42">
       <c r="A74" t="str" cm="1">
-        <f t="array" ref="A74:AL74">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A74)," ")</f>
+        <f t="array" ref="A74:AL74">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A74)," ")</f>
         <v>Card</v>
       </c>
       <c r="B74" t="str">
@@ -23867,7 +23867,7 @@
     </row>
     <row r="75" spans="1:42">
       <c r="A75" t="str" cm="1">
-        <f t="array" ref="A75:AL75">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A75)," ")</f>
+        <f t="array" ref="A75:AL75">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A75)," ")</f>
         <v>Card</v>
       </c>
       <c r="B75" t="str">
@@ -23992,7 +23992,7 @@
     </row>
     <row r="76" spans="1:42">
       <c r="A76" t="str" cm="1">
-        <f t="array" ref="A76:AL76">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A76)," ")</f>
+        <f t="array" ref="A76:AL76">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A76)," ")</f>
         <v>Card</v>
       </c>
       <c r="B76" t="str">
@@ -24117,7 +24117,7 @@
     </row>
     <row r="77" spans="1:42">
       <c r="A77" t="str" cm="1">
-        <f t="array" ref="A77:AL77">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A77)," ")</f>
+        <f t="array" ref="A77:AL77">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A77)," ")</f>
         <v>Card</v>
       </c>
       <c r="B77" t="str">
@@ -24242,7 +24242,7 @@
     </row>
     <row r="78" spans="1:42">
       <c r="A78" t="str" cm="1">
-        <f t="array" ref="A78:AL78">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A78)," ")</f>
+        <f t="array" ref="A78:AL78">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A78)," ")</f>
         <v>Card</v>
       </c>
       <c r="B78" t="str">
@@ -24367,7 +24367,7 @@
     </row>
     <row r="79" spans="1:42">
       <c r="A79" t="str" cm="1">
-        <f t="array" ref="A79:AL79">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A79)," ")</f>
+        <f t="array" ref="A79:AL79">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A79)," ")</f>
         <v>Card</v>
       </c>
       <c r="B79" t="str">
@@ -24492,7 +24492,7 @@
     </row>
     <row r="80" spans="1:42">
       <c r="A80" t="str" cm="1">
-        <f t="array" ref="A80:AL80">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A80)," ")</f>
+        <f t="array" ref="A80:AL80">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A80)," ")</f>
         <v>Card</v>
       </c>
       <c r="B80" t="str">
@@ -24617,7 +24617,7 @@
     </row>
     <row r="81" spans="1:42">
       <c r="A81" t="str" cm="1">
-        <f t="array" ref="A81:AL81">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A81)," ")</f>
+        <f t="array" ref="A81:AL81">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A81)," ")</f>
         <v>Card</v>
       </c>
       <c r="B81" t="str">
@@ -24742,7 +24742,7 @@
     </row>
     <row r="82" spans="1:42">
       <c r="A82" t="str" cm="1">
-        <f t="array" ref="A82:AL82">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A82)," ")</f>
+        <f t="array" ref="A82:AL82">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A82)," ")</f>
         <v>Card</v>
       </c>
       <c r="B82" t="str">
@@ -24867,7 +24867,7 @@
     </row>
     <row r="83" spans="1:42">
       <c r="A83" t="str" cm="1">
-        <f t="array" ref="A83:AL83">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A83)," ")</f>
+        <f t="array" ref="A83:AL83">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A83)," ")</f>
         <v>Card</v>
       </c>
       <c r="B83" t="str">
@@ -24992,7 +24992,7 @@
     </row>
     <row r="84" spans="1:42">
       <c r="A84" t="str" cm="1">
-        <f t="array" ref="A84:AL84">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A84)," ")</f>
+        <f t="array" ref="A84:AL84">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A84)," ")</f>
         <v>Card</v>
       </c>
       <c r="B84" t="str">
@@ -25117,7 +25117,7 @@
     </row>
     <row r="85" spans="1:42">
       <c r="A85" t="str" cm="1">
-        <f t="array" ref="A85:AL85">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A85)," ")</f>
+        <f t="array" ref="A85:AL85">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A85)," ")</f>
         <v>Card</v>
       </c>
       <c r="B85" t="str">
@@ -25242,7 +25242,7 @@
     </row>
     <row r="86" spans="1:42">
       <c r="A86" t="str" cm="1">
-        <f t="array" ref="A86:AL86">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A86)," ")</f>
+        <f t="array" ref="A86:AL86">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A86)," ")</f>
         <v>Card</v>
       </c>
       <c r="B86" t="str">
@@ -25367,7 +25367,7 @@
     </row>
     <row r="87" spans="1:42">
       <c r="A87" t="str" cm="1">
-        <f t="array" ref="A87:AL87">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A87)," ")</f>
+        <f t="array" ref="A87:AL87">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A87)," ")</f>
         <v>Card</v>
       </c>
       <c r="B87" t="str">
@@ -25492,7 +25492,7 @@
     </row>
     <row r="88" spans="1:42">
       <c r="A88" t="str" cm="1">
-        <f t="array" ref="A88:AL88">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A88)," ")</f>
+        <f t="array" ref="A88:AL88">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A88)," ")</f>
         <v>Card</v>
       </c>
       <c r="B88" t="str">
@@ -25617,7 +25617,7 @@
     </row>
     <row r="89" spans="1:42">
       <c r="A89" t="str" cm="1">
-        <f t="array" ref="A89:AL89">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A89)," ")</f>
+        <f t="array" ref="A89:AL89">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A89)," ")</f>
         <v>Card</v>
       </c>
       <c r="B89" t="str">
@@ -25742,7 +25742,7 @@
     </row>
     <row r="90" spans="1:42">
       <c r="A90" t="str" cm="1">
-        <f t="array" ref="A90:AL90">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A90)," ")</f>
+        <f t="array" ref="A90:AL90">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A90)," ")</f>
         <v>Card</v>
       </c>
       <c r="B90" t="str">
@@ -25867,7 +25867,7 @@
     </row>
     <row r="91" spans="1:42">
       <c r="A91" t="str" cm="1">
-        <f t="array" ref="A91:AL91">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A91)," ")</f>
+        <f t="array" ref="A91:AL91">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A91)," ")</f>
         <v>Card</v>
       </c>
       <c r="B91" t="str">
@@ -25992,7 +25992,7 @@
     </row>
     <row r="92" spans="1:42">
       <c r="A92" t="str" cm="1">
-        <f t="array" ref="A92:AL92">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A92)," ")</f>
+        <f t="array" ref="A92:AL92">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A92)," ")</f>
         <v>Card</v>
       </c>
       <c r="B92" t="str">
@@ -26117,7 +26117,7 @@
     </row>
     <row r="93" spans="1:42">
       <c r="A93" t="str" cm="1">
-        <f t="array" ref="A93:AL93">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A93)," ")</f>
+        <f t="array" ref="A93:AL93">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A93)," ")</f>
         <v>Card</v>
       </c>
       <c r="B93" t="str">
@@ -26242,7 +26242,7 @@
     </row>
     <row r="94" spans="1:42">
       <c r="A94" t="str" cm="1">
-        <f t="array" ref="A94:AL94">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A94)," ")</f>
+        <f t="array" ref="A94:AL94">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A94)," ")</f>
         <v>Card</v>
       </c>
       <c r="B94" t="str">
@@ -26367,7 +26367,7 @@
     </row>
     <row r="95" spans="1:42">
       <c r="A95" t="str" cm="1">
-        <f t="array" ref="A95:AL95">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A95)," ")</f>
+        <f t="array" ref="A95:AL95">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A95)," ")</f>
         <v>Card</v>
       </c>
       <c r="B95" t="str">
@@ -26492,7 +26492,7 @@
     </row>
     <row r="96" spans="1:42">
       <c r="A96" t="str" cm="1">
-        <f t="array" ref="A96:AL96">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A96)," ")</f>
+        <f t="array" ref="A96:AL96">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A96)," ")</f>
         <v>Card</v>
       </c>
       <c r="B96" t="str">
@@ -26617,7 +26617,7 @@
     </row>
     <row r="97" spans="1:42">
       <c r="A97" t="str" cm="1">
-        <f t="array" ref="A97:AL97">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A97)," ")</f>
+        <f t="array" ref="A97:AL97">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A97)," ")</f>
         <v>Card</v>
       </c>
       <c r="B97" t="str">
@@ -26742,7 +26742,7 @@
     </row>
     <row r="98" spans="1:42">
       <c r="A98" t="str" cm="1">
-        <f t="array" ref="A98:AL98">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A98)," ")</f>
+        <f t="array" ref="A98:AL98">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A98)," ")</f>
         <v>Card</v>
       </c>
       <c r="B98" t="str">
@@ -26867,7 +26867,7 @@
     </row>
     <row r="99" spans="1:42">
       <c r="A99" t="str" cm="1">
-        <f t="array" ref="A99:AL99">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A99)," ")</f>
+        <f t="array" ref="A99:AL99">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A99)," ")</f>
         <v>Card</v>
       </c>
       <c r="B99" t="str">
@@ -26992,7 +26992,7 @@
     </row>
     <row r="100" spans="1:42">
       <c r="A100" t="str" cm="1">
-        <f t="array" ref="A100:AL100">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A100)," ")</f>
+        <f t="array" ref="A100:AL100">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A100)," ")</f>
         <v>Card</v>
       </c>
       <c r="B100" t="str">
@@ -27117,7 +27117,7 @@
     </row>
     <row r="101" spans="1:42">
       <c r="A101" t="str" cm="1">
-        <f t="array" ref="A101:AL101">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A101)," ")</f>
+        <f t="array" ref="A101:AL101">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A101)," ")</f>
         <v>Card</v>
       </c>
       <c r="B101" t="str">
@@ -27242,7 +27242,7 @@
     </row>
     <row r="102" spans="1:42">
       <c r="A102" t="str" cm="1">
-        <f t="array" ref="A102:AL102">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A102)," ")</f>
+        <f t="array" ref="A102:AL102">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A102)," ")</f>
         <v>Card</v>
       </c>
       <c r="B102" t="str">
@@ -27367,7 +27367,7 @@
     </row>
     <row r="103" spans="1:42">
       <c r="A103" t="str" cm="1">
-        <f t="array" ref="A103:AL103">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A103)," ")</f>
+        <f t="array" ref="A103:AL103">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A103)," ")</f>
         <v>Card</v>
       </c>
       <c r="B103" t="str">
@@ -27492,7 +27492,7 @@
     </row>
     <row r="104" spans="1:42">
       <c r="A104" t="str" cm="1">
-        <f t="array" ref="A104:AL104">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A104)," ")</f>
+        <f t="array" ref="A104:AL104">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A104)," ")</f>
         <v>Card</v>
       </c>
       <c r="B104" t="str">
@@ -27617,7 +27617,7 @@
     </row>
     <row r="105" spans="1:42">
       <c r="A105" t="str" cm="1">
-        <f t="array" ref="A105:AL105">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A105)," ")</f>
+        <f t="array" ref="A105:AL105">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A105)," ")</f>
         <v>Card</v>
       </c>
       <c r="B105" t="str">
@@ -27742,7 +27742,7 @@
     </row>
     <row r="106" spans="1:42">
       <c r="A106" t="str" cm="1">
-        <f t="array" ref="A106:AL106">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A106)," ")</f>
+        <f t="array" ref="A106:AL106">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A106)," ")</f>
         <v>Card</v>
       </c>
       <c r="B106" t="str">
@@ -27867,7 +27867,7 @@
     </row>
     <row r="107" spans="1:42">
       <c r="A107" t="str" cm="1">
-        <f t="array" ref="A107:AL107">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A107)," ")</f>
+        <f t="array" ref="A107:AL107">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A107)," ")</f>
         <v>Card</v>
       </c>
       <c r="B107" t="str">
@@ -27992,7 +27992,7 @@
     </row>
     <row r="108" spans="1:42">
       <c r="A108" t="str" cm="1">
-        <f t="array" ref="A108:AL108">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A108)," ")</f>
+        <f t="array" ref="A108:AL108">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A108)," ")</f>
         <v>Card</v>
       </c>
       <c r="B108" t="str">
@@ -28117,7 +28117,7 @@
     </row>
     <row r="109" spans="1:42">
       <c r="A109" t="str" cm="1">
-        <f t="array" ref="A109:AL109">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A109)," ")</f>
+        <f t="array" ref="A109:AL109">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A109)," ")</f>
         <v>Card</v>
       </c>
       <c r="B109" t="str">
@@ -28242,7 +28242,7 @@
     </row>
     <row r="110" spans="1:42">
       <c r="A110" t="str" cm="1">
-        <f t="array" ref="A110:AL110">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A110)," ")</f>
+        <f t="array" ref="A110:AL110">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A110)," ")</f>
         <v>Card</v>
       </c>
       <c r="B110" t="str">
@@ -28367,7 +28367,7 @@
     </row>
     <row r="111" spans="1:42">
       <c r="A111" t="str" cm="1">
-        <f t="array" ref="A111:AL111">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A111)," ")</f>
+        <f t="array" ref="A111:AL111">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A111)," ")</f>
         <v>Card</v>
       </c>
       <c r="B111" t="str">
@@ -28492,7 +28492,7 @@
     </row>
     <row r="112" spans="1:42">
       <c r="A112" t="str" cm="1">
-        <f t="array" ref="A112:AL112">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A112)," ")</f>
+        <f t="array" ref="A112:AL112">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A112)," ")</f>
         <v>Card</v>
       </c>
       <c r="B112" t="str">
@@ -28617,7 +28617,7 @@
     </row>
     <row r="113" spans="1:42">
       <c r="A113" t="str" cm="1">
-        <f t="array" ref="A113:AL113">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A113)," ")</f>
+        <f t="array" ref="A113:AL113">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A113)," ")</f>
         <v>Card</v>
       </c>
       <c r="B113" t="str">
@@ -28742,7 +28742,7 @@
     </row>
     <row r="114" spans="1:42">
       <c r="A114" t="str" cm="1">
-        <f t="array" ref="A114:AL114">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A114)," ")</f>
+        <f t="array" ref="A114:AL114">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A114)," ")</f>
         <v>Card</v>
       </c>
       <c r="B114" t="str">
@@ -28867,7 +28867,7 @@
     </row>
     <row r="115" spans="1:42">
       <c r="A115" t="str" cm="1">
-        <f t="array" ref="A115:AL115">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A115)," ")</f>
+        <f t="array" ref="A115:AL115">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A115)," ")</f>
         <v>Card</v>
       </c>
       <c r="B115" t="str">
@@ -28992,7 +28992,7 @@
     </row>
     <row r="116" spans="1:42">
       <c r="A116" t="str" cm="1">
-        <f t="array" ref="A116:AL116">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A116)," ")</f>
+        <f t="array" ref="A116:AL116">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A116)," ")</f>
         <v>Card</v>
       </c>
       <c r="B116" t="str">
@@ -29117,7 +29117,7 @@
     </row>
     <row r="117" spans="1:42">
       <c r="A117" t="str" cm="1">
-        <f t="array" ref="A117:AL117">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A117)," ")</f>
+        <f t="array" ref="A117:AL117">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A117)," ")</f>
         <v>Card</v>
       </c>
       <c r="B117" t="str">
@@ -29242,7 +29242,7 @@
     </row>
     <row r="118" spans="1:42">
       <c r="A118" t="str" cm="1">
-        <f t="array" ref="A118:AL118">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A118)," ")</f>
+        <f t="array" ref="A118:AL118">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A118)," ")</f>
         <v>Card</v>
       </c>
       <c r="B118" t="str">
@@ -29367,7 +29367,7 @@
     </row>
     <row r="119" spans="1:42">
       <c r="A119" t="str" cm="1">
-        <f t="array" ref="A119:AL119">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A119)," ")</f>
+        <f t="array" ref="A119:AL119">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A119)," ")</f>
         <v>Card</v>
       </c>
       <c r="B119" t="str">
@@ -29492,7 +29492,7 @@
     </row>
     <row r="120" spans="1:42">
       <c r="A120" t="str" cm="1">
-        <f t="array" ref="A120:AL120">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A120)," ")</f>
+        <f t="array" ref="A120:AL120">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A120)," ")</f>
         <v>Card</v>
       </c>
       <c r="B120" t="str">
@@ -29617,7 +29617,7 @@
     </row>
     <row r="121" spans="1:42">
       <c r="A121" t="str" cm="1">
-        <f t="array" ref="A121:AL121">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A121)," ")</f>
+        <f t="array" ref="A121:AL121">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A121)," ")</f>
         <v>Card</v>
       </c>
       <c r="B121" t="str">
@@ -29742,7 +29742,7 @@
     </row>
     <row r="122" spans="1:42">
       <c r="A122" t="str" cm="1">
-        <f t="array" ref="A122:AL122">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A122)," ")</f>
+        <f t="array" ref="A122:AL122">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A122)," ")</f>
         <v>Card</v>
       </c>
       <c r="B122" t="str">
@@ -29867,7 +29867,7 @@
     </row>
     <row r="123" spans="1:42">
       <c r="A123" t="str" cm="1">
-        <f t="array" ref="A123:AL123">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A123)," ")</f>
+        <f t="array" ref="A123:AL123">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A123)," ")</f>
         <v>Card</v>
       </c>
       <c r="B123" t="str">
@@ -29992,7 +29992,7 @@
     </row>
     <row r="124" spans="1:42">
       <c r="A124" t="str" cm="1">
-        <f t="array" ref="A124:AL124">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A124)," ")</f>
+        <f t="array" ref="A124:AL124">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A124)," ")</f>
         <v>Card</v>
       </c>
       <c r="B124" t="str">
@@ -30117,7 +30117,7 @@
     </row>
     <row r="125" spans="1:42">
       <c r="A125" t="str" cm="1">
-        <f t="array" ref="A125:AL125">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A125)," ")</f>
+        <f t="array" ref="A125:AL125">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A125)," ")</f>
         <v>Card</v>
       </c>
       <c r="B125" t="str">
@@ -30242,7 +30242,7 @@
     </row>
     <row r="126" spans="1:42">
       <c r="A126" t="str" cm="1">
-        <f t="array" ref="A126:AL126">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A126)," ")</f>
+        <f t="array" ref="A126:AL126">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A126)," ")</f>
         <v>Card</v>
       </c>
       <c r="B126" t="str">
@@ -30367,7 +30367,7 @@
     </row>
     <row r="127" spans="1:42">
       <c r="A127" t="str" cm="1">
-        <f t="array" ref="A127:AL127">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A127)," ")</f>
+        <f t="array" ref="A127:AL127">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A127)," ")</f>
         <v>Card</v>
       </c>
       <c r="B127" t="str">
@@ -30492,7 +30492,7 @@
     </row>
     <row r="128" spans="1:42">
       <c r="A128" t="str" cm="1">
-        <f t="array" ref="A128:AL128">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A128)," ")</f>
+        <f t="array" ref="A128:AL128">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A128)," ")</f>
         <v>Card</v>
       </c>
       <c r="B128" t="str">
@@ -30617,7 +30617,7 @@
     </row>
     <row r="129" spans="1:42">
       <c r="A129" t="str" cm="1">
-        <f t="array" ref="A129:AL129">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A129)," ")</f>
+        <f t="array" ref="A129:AL129">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A129)," ")</f>
         <v>Card</v>
       </c>
       <c r="B129" t="str">
@@ -30742,7 +30742,7 @@
     </row>
     <row r="130" spans="1:42">
       <c r="A130" t="str" cm="1">
-        <f t="array" ref="A130:AL130">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A130)," ")</f>
+        <f t="array" ref="A130:AL130">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A130)," ")</f>
         <v>Card</v>
       </c>
       <c r="B130" t="str">
@@ -30867,7 +30867,7 @@
     </row>
     <row r="131" spans="1:42">
       <c r="A131" t="str" cm="1">
-        <f t="array" ref="A131:AL131">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A131)," ")</f>
+        <f t="array" ref="A131:AL131">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A131)," ")</f>
         <v>Card</v>
       </c>
       <c r="B131" t="str">
@@ -30992,7 +30992,7 @@
     </row>
     <row r="132" spans="1:42">
       <c r="A132" t="str" cm="1">
-        <f t="array" ref="A132:AL132">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A132)," ")</f>
+        <f t="array" ref="A132:AL132">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A132)," ")</f>
         <v>Card</v>
       </c>
       <c r="B132" t="str">
@@ -31117,7 +31117,7 @@
     </row>
     <row r="133" spans="1:42">
       <c r="A133" t="str" cm="1">
-        <f t="array" ref="A133:AL133">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A133)," ")</f>
+        <f t="array" ref="A133:AL133">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A133)," ")</f>
         <v>Card</v>
       </c>
       <c r="B133" t="str">
@@ -31242,7 +31242,7 @@
     </row>
     <row r="134" spans="1:42">
       <c r="A134" t="str" cm="1">
-        <f t="array" ref="A134:AL134">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A134)," ")</f>
+        <f t="array" ref="A134:AL134">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A134)," ")</f>
         <v>Card</v>
       </c>
       <c r="B134" t="str">
@@ -31367,7 +31367,7 @@
     </row>
     <row r="135" spans="1:42">
       <c r="A135" t="str" cm="1">
-        <f t="array" ref="A135:AL135">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A135)," ")</f>
+        <f t="array" ref="A135:AL135">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A135)," ")</f>
         <v>Card</v>
       </c>
       <c r="B135" t="str">
@@ -31492,7 +31492,7 @@
     </row>
     <row r="136" spans="1:42">
       <c r="A136" t="str" cm="1">
-        <f t="array" ref="A136:AL136">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A136)," ")</f>
+        <f t="array" ref="A136:AL136">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A136)," ")</f>
         <v>Card</v>
       </c>
       <c r="B136" t="str">
@@ -31617,7 +31617,7 @@
     </row>
     <row r="137" spans="1:42">
       <c r="A137" t="str" cm="1">
-        <f t="array" ref="A137:AL137">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A137)," ")</f>
+        <f t="array" ref="A137:AL137">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A137)," ")</f>
         <v>Card</v>
       </c>
       <c r="B137" t="str">
@@ -31742,7 +31742,7 @@
     </row>
     <row r="138" spans="1:42">
       <c r="A138" t="str" cm="1">
-        <f t="array" ref="A138:AL138">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A138)," ")</f>
+        <f t="array" ref="A138:AL138">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A138)," ")</f>
         <v>Card</v>
       </c>
       <c r="B138" t="str">
@@ -31867,7 +31867,7 @@
     </row>
     <row r="139" spans="1:42">
       <c r="A139" t="str" cm="1">
-        <f t="array" ref="A139:AL139">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A139)," ")</f>
+        <f t="array" ref="A139:AL139">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A139)," ")</f>
         <v>Card</v>
       </c>
       <c r="B139" t="str">
@@ -31992,7 +31992,7 @@
     </row>
     <row r="140" spans="1:42">
       <c r="A140" t="str" cm="1">
-        <f t="array" ref="A140:AL140">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A140)," ")</f>
+        <f t="array" ref="A140:AL140">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A140)," ")</f>
         <v>Card</v>
       </c>
       <c r="B140" t="str">
@@ -32117,7 +32117,7 @@
     </row>
     <row r="141" spans="1:42">
       <c r="A141" t="str" cm="1">
-        <f t="array" ref="A141:AL141">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A141)," ")</f>
+        <f t="array" ref="A141:AL141">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A141)," ")</f>
         <v>Card</v>
       </c>
       <c r="B141" t="str">
@@ -32242,7 +32242,7 @@
     </row>
     <row r="142" spans="1:42">
       <c r="A142" t="str" cm="1">
-        <f t="array" ref="A142:AL142">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A142)," ")</f>
+        <f t="array" ref="A142:AL142">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A142)," ")</f>
         <v>Card</v>
       </c>
       <c r="B142" t="str">
@@ -32367,7 +32367,7 @@
     </row>
     <row r="143" spans="1:42">
       <c r="A143" t="str" cm="1">
-        <f t="array" ref="A143:AL143">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A143)," ")</f>
+        <f t="array" ref="A143:AL143">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A143)," ")</f>
         <v>Card</v>
       </c>
       <c r="B143" t="str">
@@ -32492,7 +32492,7 @@
     </row>
     <row r="144" spans="1:42">
       <c r="A144" t="str" cm="1">
-        <f t="array" ref="A144:AL144">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A144)," ")</f>
+        <f t="array" ref="A144:AL144">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A144)," ")</f>
         <v>Card</v>
       </c>
       <c r="B144" t="str">
@@ -32617,7 +32617,7 @@
     </row>
     <row r="145" spans="1:42">
       <c r="A145" t="str" cm="1">
-        <f t="array" ref="A145:AL145">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A145)," ")</f>
+        <f t="array" ref="A145:AL145">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A145)," ")</f>
         <v>Card</v>
       </c>
       <c r="B145" t="str">
@@ -32742,7 +32742,7 @@
     </row>
     <row r="146" spans="1:42">
       <c r="A146" t="str" cm="1">
-        <f t="array" ref="A146:AL146">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A146)," ")</f>
+        <f t="array" ref="A146:AL146">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A146)," ")</f>
         <v>Card</v>
       </c>
       <c r="B146" t="str">
@@ -32867,7 +32867,7 @@
     </row>
     <row r="147" spans="1:42">
       <c r="A147" t="str" cm="1">
-        <f t="array" ref="A147:AL147">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A147)," ")</f>
+        <f t="array" ref="A147:AL147">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A147)," ")</f>
         <v>Card</v>
       </c>
       <c r="B147" t="str">
@@ -32992,7 +32992,7 @@
     </row>
     <row r="148" spans="1:42">
       <c r="A148" t="str" cm="1">
-        <f t="array" ref="A148:AL148">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A148)," ")</f>
+        <f t="array" ref="A148:AL148">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A148)," ")</f>
         <v>Card</v>
       </c>
       <c r="B148" t="str">
@@ -33117,7 +33117,7 @@
     </row>
     <row r="149" spans="1:42">
       <c r="A149" t="str" cm="1">
-        <f t="array" ref="A149:AL149">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A149)," ")</f>
+        <f t="array" ref="A149:AL149">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A149)," ")</f>
         <v>Card</v>
       </c>
       <c r="B149" t="str">
@@ -33242,7 +33242,7 @@
     </row>
     <row r="150" spans="1:42">
       <c r="A150" t="str" cm="1">
-        <f t="array" ref="A150:AL150">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A150)," ")</f>
+        <f t="array" ref="A150:AL150">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A150)," ")</f>
         <v>Card</v>
       </c>
       <c r="B150" t="str">
@@ -33367,7 +33367,7 @@
     </row>
     <row r="151" spans="1:42">
       <c r="A151" t="str" cm="1">
-        <f t="array" ref="A151:AL151">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A151)," ")</f>
+        <f t="array" ref="A151:AL151">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A151)," ")</f>
         <v>Card</v>
       </c>
       <c r="B151" t="str">
@@ -33492,7 +33492,7 @@
     </row>
     <row r="152" spans="1:42">
       <c r="A152" t="str" cm="1">
-        <f t="array" ref="A152:AL152">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A152)," ")</f>
+        <f t="array" ref="A152:AL152">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A152)," ")</f>
         <v>Card</v>
       </c>
       <c r="B152" t="str">
@@ -33617,7 +33617,7 @@
     </row>
     <row r="153" spans="1:42">
       <c r="A153" t="str" cm="1">
-        <f t="array" ref="A153:AL153">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A153)," ")</f>
+        <f t="array" ref="A153:AL153">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A153)," ")</f>
         <v>Card</v>
       </c>
       <c r="B153" t="str">
@@ -33742,7 +33742,7 @@
     </row>
     <row r="154" spans="1:42">
       <c r="A154" t="str" cm="1">
-        <f t="array" ref="A154:AL154">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A154)," ")</f>
+        <f t="array" ref="A154:AL154">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A154)," ")</f>
         <v>Card</v>
       </c>
       <c r="B154" t="str">
@@ -33867,7 +33867,7 @@
     </row>
     <row r="155" spans="1:42">
       <c r="A155" t="str" cm="1">
-        <f t="array" ref="A155:AL155">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A155)," ")</f>
+        <f t="array" ref="A155:AL155">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A155)," ")</f>
         <v>Card</v>
       </c>
       <c r="B155" t="str">
@@ -33992,7 +33992,7 @@
     </row>
     <row r="156" spans="1:42">
       <c r="A156" t="str" cm="1">
-        <f t="array" ref="A156:AL156">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A156)," ")</f>
+        <f t="array" ref="A156:AL156">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A156)," ")</f>
         <v>Card</v>
       </c>
       <c r="B156" t="str">
@@ -34117,7 +34117,7 @@
     </row>
     <row r="157" spans="1:42">
       <c r="A157" t="str" cm="1">
-        <f t="array" ref="A157:AL157">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A157)," ")</f>
+        <f t="array" ref="A157:AL157">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A157)," ")</f>
         <v>Card</v>
       </c>
       <c r="B157" t="str">
@@ -34242,7 +34242,7 @@
     </row>
     <row r="158" spans="1:42">
       <c r="A158" t="str" cm="1">
-        <f t="array" ref="A158:AL158">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A158)," ")</f>
+        <f t="array" ref="A158:AL158">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A158)," ")</f>
         <v>Card</v>
       </c>
       <c r="B158" t="str">
@@ -34367,7 +34367,7 @@
     </row>
     <row r="159" spans="1:42">
       <c r="A159" t="str" cm="1">
-        <f t="array" ref="A159:AL159">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A159)," ")</f>
+        <f t="array" ref="A159:AL159">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A159)," ")</f>
         <v>Card</v>
       </c>
       <c r="B159" t="str">
@@ -34492,7 +34492,7 @@
     </row>
     <row r="160" spans="1:42">
       <c r="A160" t="str" cm="1">
-        <f t="array" ref="A160:AL160">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A160)," ")</f>
+        <f t="array" ref="A160:AL160">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A160)," ")</f>
         <v>Card</v>
       </c>
       <c r="B160" t="str">
@@ -34617,7 +34617,7 @@
     </row>
     <row r="161" spans="1:42">
       <c r="A161" t="str" cm="1">
-        <f t="array" ref="A161:AL161">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A161)," ")</f>
+        <f t="array" ref="A161:AL161">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A161)," ")</f>
         <v>Card</v>
       </c>
       <c r="B161" t="str">
@@ -34742,7 +34742,7 @@
     </row>
     <row r="162" spans="1:42">
       <c r="A162" t="str" cm="1">
-        <f t="array" ref="A162:AL162">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A162)," ")</f>
+        <f t="array" ref="A162:AL162">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A162)," ")</f>
         <v>Card</v>
       </c>
       <c r="B162" t="str">
@@ -34867,7 +34867,7 @@
     </row>
     <row r="163" spans="1:42">
       <c r="A163" t="str" cm="1">
-        <f t="array" ref="A163:AL163">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A163)," ")</f>
+        <f t="array" ref="A163:AL163">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A163)," ")</f>
         <v>Card</v>
       </c>
       <c r="B163" t="str">
@@ -34992,7 +34992,7 @@
     </row>
     <row r="164" spans="1:42">
       <c r="A164" t="str" cm="1">
-        <f t="array" ref="A164:AL164">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A164)," ")</f>
+        <f t="array" ref="A164:AL164">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A164)," ")</f>
         <v>Card</v>
       </c>
       <c r="B164" t="str">
@@ -35117,7 +35117,7 @@
     </row>
     <row r="165" spans="1:42">
       <c r="A165" t="str" cm="1">
-        <f t="array" ref="A165:AL165">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A165)," ")</f>
+        <f t="array" ref="A165:AL165">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A165)," ")</f>
         <v>Card</v>
       </c>
       <c r="B165" t="str">
@@ -35242,7 +35242,7 @@
     </row>
     <row r="166" spans="1:42">
       <c r="A166" t="str" cm="1">
-        <f t="array" ref="A166:AL166">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A166)," ")</f>
+        <f t="array" ref="A166:AL166">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A166)," ")</f>
         <v>Card</v>
       </c>
       <c r="B166" t="str">
@@ -35367,7 +35367,7 @@
     </row>
     <row r="167" spans="1:42">
       <c r="A167" t="str" cm="1">
-        <f t="array" ref="A167:AL167">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A167)," ")</f>
+        <f t="array" ref="A167:AL167">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A167)," ")</f>
         <v>Card</v>
       </c>
       <c r="B167" t="str">
@@ -35492,7 +35492,7 @@
     </row>
     <row r="168" spans="1:42">
       <c r="A168" t="str" cm="1">
-        <f t="array" ref="A168:AL168">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A168)," ")</f>
+        <f t="array" ref="A168:AL168">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A168)," ")</f>
         <v>Card</v>
       </c>
       <c r="B168" t="str">
@@ -35617,7 +35617,7 @@
     </row>
     <row r="169" spans="1:42">
       <c r="A169" t="str" cm="1">
-        <f t="array" ref="A169:AL169">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A169)," ")</f>
+        <f t="array" ref="A169:AL169">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A169)," ")</f>
         <v>Card</v>
       </c>
       <c r="B169" t="str">
@@ -35742,7 +35742,7 @@
     </row>
     <row r="170" spans="1:42">
       <c r="A170" t="str" cm="1">
-        <f t="array" ref="A170:AL170">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A170)," ")</f>
+        <f t="array" ref="A170:AL170">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A170)," ")</f>
         <v>Card</v>
       </c>
       <c r="B170" t="str">
@@ -35867,7 +35867,7 @@
     </row>
     <row r="171" spans="1:42">
       <c r="A171" t="str" cm="1">
-        <f t="array" ref="A171:AL171">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A171)," ")</f>
+        <f t="array" ref="A171:AL171">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A171)," ")</f>
         <v>Card</v>
       </c>
       <c r="B171" t="str">
@@ -35992,7 +35992,7 @@
     </row>
     <row r="172" spans="1:42">
       <c r="A172" t="str" cm="1">
-        <f t="array" ref="A172:AL172">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A172)," ")</f>
+        <f t="array" ref="A172:AL172">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A172)," ")</f>
         <v>Card</v>
       </c>
       <c r="B172" t="str">
@@ -36117,7 +36117,7 @@
     </row>
     <row r="173" spans="1:42">
       <c r="A173" t="str" cm="1">
-        <f t="array" ref="A173:AL173">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A173)," ")</f>
+        <f t="array" ref="A173:AL173">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A173)," ")</f>
         <v>Card</v>
       </c>
       <c r="B173" t="str">
@@ -36242,7 +36242,7 @@
     </row>
     <row r="174" spans="1:42">
       <c r="A174" t="str" cm="1">
-        <f t="array" ref="A174:AL174">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A174)," ")</f>
+        <f t="array" ref="A174:AL174">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A174)," ")</f>
         <v>Card</v>
       </c>
       <c r="B174" t="str">
@@ -36367,7 +36367,7 @@
     </row>
     <row r="175" spans="1:42">
       <c r="A175" t="str" cm="1">
-        <f t="array" ref="A175:AL175">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A175)," ")</f>
+        <f t="array" ref="A175:AL175">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A175)," ")</f>
         <v>Card</v>
       </c>
       <c r="B175" t="str">
@@ -36492,7 +36492,7 @@
     </row>
     <row r="176" spans="1:42">
       <c r="A176" t="str" cm="1">
-        <f t="array" ref="A176:AL176">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A176)," ")</f>
+        <f t="array" ref="A176:AL176">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A176)," ")</f>
         <v>Card</v>
       </c>
       <c r="B176" t="str">
@@ -36617,7 +36617,7 @@
     </row>
     <row r="177" spans="1:42">
       <c r="A177" t="str" cm="1">
-        <f t="array" ref="A177:AL177">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A177)," ")</f>
+        <f t="array" ref="A177:AL177">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A177)," ")</f>
         <v>Card</v>
       </c>
       <c r="B177" t="str">
@@ -36742,7 +36742,7 @@
     </row>
     <row r="178" spans="1:42">
       <c r="A178" t="str" cm="1">
-        <f t="array" ref="A178:AL178">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A178)," ")</f>
+        <f t="array" ref="A178:AL178">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A178)," ")</f>
         <v>Card</v>
       </c>
       <c r="B178" t="str">
@@ -36867,7 +36867,7 @@
     </row>
     <row r="179" spans="1:42">
       <c r="A179" t="str" cm="1">
-        <f t="array" ref="A179:AL179">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A179)," ")</f>
+        <f t="array" ref="A179:AL179">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A179)," ")</f>
         <v>Card</v>
       </c>
       <c r="B179" t="str">
@@ -36992,7 +36992,7 @@
     </row>
     <row r="180" spans="1:42">
       <c r="A180" t="str" cm="1">
-        <f t="array" ref="A180:AL180">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A180)," ")</f>
+        <f t="array" ref="A180:AL180">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A180)," ")</f>
         <v>Card</v>
       </c>
       <c r="B180" t="str">
@@ -37117,7 +37117,7 @@
     </row>
     <row r="181" spans="1:42">
       <c r="A181" t="str" cm="1">
-        <f t="array" ref="A181:AL181">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A181)," ")</f>
+        <f t="array" ref="A181:AL181">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A181)," ")</f>
         <v>Card</v>
       </c>
       <c r="B181" t="str">
@@ -37242,7 +37242,7 @@
     </row>
     <row r="182" spans="1:42">
       <c r="A182" t="str" cm="1">
-        <f t="array" ref="A182:AL182">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A182)," ")</f>
+        <f t="array" ref="A182:AL182">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A182)," ")</f>
         <v>Card</v>
       </c>
       <c r="B182" t="str">
@@ -37367,7 +37367,7 @@
     </row>
     <row r="183" spans="1:42">
       <c r="A183" t="str" cm="1">
-        <f t="array" ref="A183:AL183">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A183)," ")</f>
+        <f t="array" ref="A183:AL183">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A183)," ")</f>
         <v>Card</v>
       </c>
       <c r="B183" t="str">
@@ -37492,7 +37492,7 @@
     </row>
     <row r="184" spans="1:42">
       <c r="A184" t="str" cm="1">
-        <f t="array" ref="A184:AL184">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A184)," ")</f>
+        <f t="array" ref="A184:AL184">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A184)," ")</f>
         <v>Card</v>
       </c>
       <c r="B184" t="str">
@@ -37617,7 +37617,7 @@
     </row>
     <row r="185" spans="1:42">
       <c r="A185" t="str" cm="1">
-        <f t="array" ref="A185:AL185">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A185)," ")</f>
+        <f t="array" ref="A185:AL185">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A185)," ")</f>
         <v>Card</v>
       </c>
       <c r="B185" t="str">
@@ -37742,7 +37742,7 @@
     </row>
     <row r="186" spans="1:42">
       <c r="A186" t="str" cm="1">
-        <f t="array" ref="A186:AL186">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A186)," ")</f>
+        <f t="array" ref="A186:AL186">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A186)," ")</f>
         <v>Card</v>
       </c>
       <c r="B186" t="str">
@@ -37867,7 +37867,7 @@
     </row>
     <row r="187" spans="1:42">
       <c r="A187" t="str" cm="1">
-        <f t="array" ref="A187:AL187">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A187)," ")</f>
+        <f t="array" ref="A187:AL187">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A187)," ")</f>
         <v>Card</v>
       </c>
       <c r="B187" t="str">
@@ -37992,7 +37992,7 @@
     </row>
     <row r="188" spans="1:42">
       <c r="A188" t="str" cm="1">
-        <f t="array" ref="A188:AL188">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A188)," ")</f>
+        <f t="array" ref="A188:AL188">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A188)," ")</f>
         <v>Card</v>
       </c>
       <c r="B188" t="str">
@@ -38117,7 +38117,7 @@
     </row>
     <row r="189" spans="1:42">
       <c r="A189" t="str" cm="1">
-        <f t="array" ref="A189:AL189">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A189)," ")</f>
+        <f t="array" ref="A189:AL189">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A189)," ")</f>
         <v>Card</v>
       </c>
       <c r="B189" t="str">
@@ -38242,7 +38242,7 @@
     </row>
     <row r="190" spans="1:42">
       <c r="A190" t="str" cm="1">
-        <f t="array" ref="A190:AL190">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A190)," ")</f>
+        <f t="array" ref="A190:AL190">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A190)," ")</f>
         <v>Card</v>
       </c>
       <c r="B190" t="str">
@@ -38367,7 +38367,7 @@
     </row>
     <row r="191" spans="1:42">
       <c r="A191" t="str" cm="1">
-        <f t="array" ref="A191:AL191">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A191)," ")</f>
+        <f t="array" ref="A191:AL191">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A191)," ")</f>
         <v>Card</v>
       </c>
       <c r="B191" t="str">
@@ -38492,7 +38492,7 @@
     </row>
     <row r="192" spans="1:42">
       <c r="A192" t="str" cm="1">
-        <f t="array" ref="A192:AL192">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A192)," ")</f>
+        <f t="array" ref="A192:AL192">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A192)," ")</f>
         <v>Card</v>
       </c>
       <c r="B192" t="str">
@@ -38617,7 +38617,7 @@
     </row>
     <row r="193" spans="1:42">
       <c r="A193" t="str" cm="1">
-        <f t="array" ref="A193:AL193">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A193)," ")</f>
+        <f t="array" ref="A193:AL193">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A193)," ")</f>
         <v>Card</v>
       </c>
       <c r="B193" t="str">
@@ -38742,7 +38742,7 @@
     </row>
     <row r="194" spans="1:42">
       <c r="A194" t="str" cm="1">
-        <f t="array" ref="A194:AL194">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A194)," ")</f>
+        <f t="array" ref="A194:AL194">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A194)," ")</f>
         <v>Card</v>
       </c>
       <c r="B194" t="str">
@@ -38867,7 +38867,7 @@
     </row>
     <row r="195" spans="1:42">
       <c r="A195" t="str" cm="1">
-        <f t="array" ref="A195:AL195">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A195)," ")</f>
+        <f t="array" ref="A195:AL195">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A195)," ")</f>
         <v>Card</v>
       </c>
       <c r="B195" t="str">
@@ -38992,7 +38992,7 @@
     </row>
     <row r="196" spans="1:42">
       <c r="A196" t="str" cm="1">
-        <f t="array" ref="A196:AL196">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A196)," ")</f>
+        <f t="array" ref="A196:AL196">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A196)," ")</f>
         <v>Card</v>
       </c>
       <c r="B196" t="str">
@@ -39117,7 +39117,7 @@
     </row>
     <row r="197" spans="1:42">
       <c r="A197" t="str" cm="1">
-        <f t="array" ref="A197:AL197">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A197)," ")</f>
+        <f t="array" ref="A197:AL197">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A197)," ")</f>
         <v>Card</v>
       </c>
       <c r="B197" t="str">
@@ -39242,7 +39242,7 @@
     </row>
     <row r="198" spans="1:42">
       <c r="A198" t="str" cm="1">
-        <f t="array" ref="A198:AL198">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A198)," ")</f>
+        <f t="array" ref="A198:AL198">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A198)," ")</f>
         <v>Card</v>
       </c>
       <c r="B198" t="str">
@@ -39367,7 +39367,7 @@
     </row>
     <row r="199" spans="1:42">
       <c r="A199" t="str" cm="1">
-        <f t="array" ref="A199:AL199">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A199)," ")</f>
+        <f t="array" ref="A199:AL199">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A199)," ")</f>
         <v>Card</v>
       </c>
       <c r="B199" t="str">
@@ -39492,7 +39492,7 @@
     </row>
     <row r="200" spans="1:42">
       <c r="A200" t="str" cm="1">
-        <f t="array" ref="A200:AL200">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A200)," ")</f>
+        <f t="array" ref="A200:AL200">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A200)," ")</f>
         <v>Card</v>
       </c>
       <c r="B200" t="str">
@@ -39617,7 +39617,7 @@
     </row>
     <row r="201" spans="1:42">
       <c r="A201" t="str" cm="1">
-        <f t="array" ref="A201:AL201">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A201)," ")</f>
+        <f t="array" ref="A201:AL201">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A201)," ")</f>
         <v>Card</v>
       </c>
       <c r="B201" t="str">
@@ -39742,7 +39742,7 @@
     </row>
     <row r="202" spans="1:42">
       <c r="A202" t="str" cm="1">
-        <f t="array" ref="A202:AL202">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A202)," ")</f>
+        <f t="array" ref="A202:AL202">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A202)," ")</f>
         <v>Card</v>
       </c>
       <c r="B202" t="str">
@@ -39867,7 +39867,7 @@
     </row>
     <row r="203" spans="1:42">
       <c r="A203" t="str" cm="1">
-        <f t="array" ref="A203:AL203">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A203)," ")</f>
+        <f t="array" ref="A203:AL203">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A203)," ")</f>
         <v>Card</v>
       </c>
       <c r="B203" t="str">
@@ -39992,7 +39992,7 @@
     </row>
     <row r="204" spans="1:42">
       <c r="A204" t="str" cm="1">
-        <f t="array" ref="A204:AL204">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A204)," ")</f>
+        <f t="array" ref="A204:AL204">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A204)," ")</f>
         <v>Card</v>
       </c>
       <c r="B204" t="str">
@@ -40117,7 +40117,7 @@
     </row>
     <row r="205" spans="1:42">
       <c r="A205" t="str" cm="1">
-        <f t="array" ref="A205:AL205">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A205)," ")</f>
+        <f t="array" ref="A205:AL205">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A205)," ")</f>
         <v>Card</v>
       </c>
       <c r="B205" t="str">
@@ -40242,7 +40242,7 @@
     </row>
     <row r="206" spans="1:42">
       <c r="A206" t="str" cm="1">
-        <f t="array" ref="A206:AL206">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A206)," ")</f>
+        <f t="array" ref="A206:AL206">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A206)," ")</f>
         <v>Card</v>
       </c>
       <c r="B206" t="str">
@@ -40367,7 +40367,7 @@
     </row>
     <row r="207" spans="1:42">
       <c r="A207" t="str" cm="1">
-        <f t="array" ref="A207:AL207">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A207)," ")</f>
+        <f t="array" ref="A207:AL207">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A207)," ")</f>
         <v>Card</v>
       </c>
       <c r="B207" t="str">
@@ -40492,7 +40492,7 @@
     </row>
     <row r="208" spans="1:42">
       <c r="A208" t="str" cm="1">
-        <f t="array" ref="A208:AL208">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A208)," ")</f>
+        <f t="array" ref="A208:AL208">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A208)," ")</f>
         <v>Card</v>
       </c>
       <c r="B208" t="str">
@@ -40617,7 +40617,7 @@
     </row>
     <row r="209" spans="1:42">
       <c r="A209" t="str" cm="1">
-        <f t="array" ref="A209:AL209">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A209)," ")</f>
+        <f t="array" ref="A209:AL209">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A209)," ")</f>
         <v>Card</v>
       </c>
       <c r="B209" t="str">
@@ -40742,7 +40742,7 @@
     </row>
     <row r="210" spans="1:42">
       <c r="A210" t="str" cm="1">
-        <f t="array" ref="A210:AL210">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A210)," ")</f>
+        <f t="array" ref="A210:AL210">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A210)," ")</f>
         <v>Card</v>
       </c>
       <c r="B210" t="str">
@@ -40867,7 +40867,7 @@
     </row>
     <row r="211" spans="1:42">
       <c r="A211" t="str" cm="1">
-        <f t="array" ref="A211:AL211">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A211)," ")</f>
+        <f t="array" ref="A211:AL211">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A211)," ")</f>
         <v>Card</v>
       </c>
       <c r="B211" t="str">
@@ -40992,7 +40992,7 @@
     </row>
     <row r="212" spans="1:42">
       <c r="A212" t="str" cm="1">
-        <f t="array" ref="A212:AL212">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A212)," ")</f>
+        <f t="array" ref="A212:AL212">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A212)," ")</f>
         <v>Card</v>
       </c>
       <c r="B212" t="str">
@@ -41117,7 +41117,7 @@
     </row>
     <row r="213" spans="1:42">
       <c r="A213" t="str" cm="1">
-        <f t="array" ref="A213:AL213">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A213)," ")</f>
+        <f t="array" ref="A213:AL213">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A213)," ")</f>
         <v>Card</v>
       </c>
       <c r="B213" t="str">
@@ -41242,7 +41242,7 @@
     </row>
     <row r="214" spans="1:42">
       <c r="A214" t="str" cm="1">
-        <f t="array" ref="A214:AL214">_xlfn.TEXTSPLIT(TRIM('D2-Input'!A214)," ")</f>
+        <f t="array" ref="A214:AL214">_xlfn.TEXTSPLIT(TRIM('D4-Input'!A214)," ")</f>
         <v>Card</v>
       </c>
       <c r="B214" t="str">
@@ -41378,8 +41378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374BA9AD-E087-40DC-9BD6-32F317CC1C8D}">
   <dimension ref="A1:A214"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>